<commit_message>
Trying to fix logic and uncertainties propagation after Tuning Corrector in gas mixture
After a very large amount of hassle, including propagating the uncertainties and fixing the clearZeros usage in some places, the output finally looks fine.
</commit_message>
<xml_diff>
--- a/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
+++ b/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7ar\Documents\Programs\180911MSRESOLVESG\MSRESOLVESG36.34ARogers\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\MSRESOLVESG\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83012BCB-DD04-44E4-9DFA-E3D0460BAFC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1903,8 +1907,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>22411</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -2167,7 +2171,7 @@
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
-                                    <m:t>135</m:t>
+                                    <m:t>155</m:t>
                                   </m:r>
                                 </m:den>
                               </m:f>
@@ -2286,7 +2290,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -2349,65 +2353,23 @@
                     </a:schemeClr>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝑇_𝑀𝑆</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:effectLst/>
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> (</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝑚</a:t>
+                <a:t>𝑇_𝑀𝑆 (𝑚)</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1600" b="0" i="0">
                   <a:solidFill>
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="dk1"/>
                   </a:solidFill>
                   <a:effectLst/>
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>= {█(〖10〗^((30−𝑚/135))      𝑚&gt;30@1                      𝑚</a:t>
+                <a:t>= {█(10^((30−𝑚/155))      𝑚&gt;30@1                      𝑚</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1600" b="0" i="0">
@@ -2954,8 +2916,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -3594,7 +3556,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -6101,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
MadixKo Update. Added New "IF THEN" Function & Clarification Comment Added
</commit_message>
<xml_diff>
--- a/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
+++ b/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\MSRESOLVESG\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Github/MSRESOLVESG/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D0C7CFB-F7A1-46F2-975D-ABE12E056E6F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26445" yWindow="180" windowWidth="22605" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>Species</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>See yellow highlighted table at end.</t>
+  </si>
+  <si>
+    <t>The below table(s) were manually populated from the above table.</t>
   </si>
 </sst>
 </file>
@@ -1907,8 +1910,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>22411</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -2290,7 +2293,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -6061,10 +6064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T75"/>
+  <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6635,44 +6638,51 @@
         <v>15</v>
       </c>
       <c r="C28" s="6">
-        <f>10^((30-C11)/155)</f>
+        <f>IF(C27&lt;30,1,10^((30-C11)/155))</f>
         <v>0.640400427119728</v>
       </c>
       <c r="D28" s="6">
-        <f>10^((30-D11)/155)</f>
+        <f t="shared" ref="D28:N28" si="1">IF(D27&lt;30,1,10^((30-D11)/155))</f>
         <v>0.81222699470800896</v>
       </c>
       <c r="E28" s="6">
-        <f>10^((30-E11)/155)</f>
+        <f t="shared" si="1"/>
         <v>0.95641231880567645</v>
       </c>
       <c r="F28" s="6">
-        <f>10^((30-F11)/155)</f>
+        <f t="shared" si="1"/>
         <v>0.9707262508693274</v>
       </c>
       <c r="G28" s="6">
-        <f>10^((30-G11)/155)</f>
+        <f t="shared" si="1"/>
         <v>0.98525440921080254</v>
       </c>
       <c r="H28" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I28" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J28" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K28" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L28" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M28" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N28" s="6">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O28" s="17"/>
@@ -6724,51 +6734,51 @@
         <v>14</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" ref="C36:N36" si="1">+(28/C11)^(0.5)</f>
+        <f t="shared" ref="C36:N36" si="2">+(28/C11)^(0.5)</f>
         <v>0.68313005106397318</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.7977240352174656</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92113237294367656</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.93541434669348533</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95038192662298293</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96609178307929588</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98260736888103495</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.247219128924647</v>
       </c>
       <c r="L36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3228756555322954</v>
       </c>
       <c r="M36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3662601021279464</v>
       </c>
       <c r="N36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="O36" s="4"/>
@@ -6827,51 +6837,51 @@
         <v>6</v>
       </c>
       <c r="C42" s="11">
-        <f t="shared" ref="C42:N42" si="2">+C12/(C$28*C$36)</f>
+        <f t="shared" ref="C42:N42" si="3">+C12/(C$28*C$36)</f>
         <v>68.575068696001424</v>
       </c>
       <c r="D42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44.05134678050878</v>
       </c>
       <c r="G42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106.79562068249264</v>
       </c>
       <c r="H42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.386081729148845</v>
       </c>
       <c r="I42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>69.203633265478615</v>
       </c>
       <c r="J42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="K42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21.957751641341996</v>
       </c>
       <c r="N42" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P42" s="28" t="s">
@@ -6887,58 +6897,58 @@
         <v>9</v>
       </c>
       <c r="C43" s="11">
-        <f t="shared" ref="C43:N43" si="3">+C13/(C$28*C$36)</f>
+        <f t="shared" ref="C43:N43" si="4">+C13/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89.672625238771516</v>
       </c>
       <c r="F43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110.12836695127194</v>
       </c>
       <c r="G43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.2038686204747795</v>
       </c>
       <c r="H43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.3158850511217821</v>
       </c>
       <c r="I43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18.318608805567866</v>
       </c>
       <c r="J43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.3192505471139997</v>
       </c>
       <c r="N43" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P43" s="10" t="s">
         <v>9</v>
       </c>
       <c r="Q43">
-        <f t="shared" ref="Q43:Q47" si="4">+SUM(C43:N43)</f>
+        <f t="shared" ref="Q43:Q47" si="5">+SUM(C43:N43)</f>
         <v>237.95860521432189</v>
       </c>
     </row>
@@ -6947,58 +6957,58 @@
         <v>8</v>
       </c>
       <c r="C44" s="11">
-        <f t="shared" ref="C44:N44" si="5">+C14/(C$28*C$36)</f>
+        <f t="shared" ref="C44:N44" si="6">+C14/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79.292424204915804</v>
       </c>
       <c r="G44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>106.79562068249264</v>
       </c>
       <c r="H44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.1052950170405942</v>
       </c>
       <c r="I44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42.743420546325019</v>
       </c>
       <c r="J44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="K44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M44" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N44" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P44" s="10" t="s">
         <v>8</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>240.93676045077405</v>
       </c>
     </row>
@@ -7007,58 +7017,58 @@
         <v>5</v>
       </c>
       <c r="C45" s="11">
-        <f t="shared" ref="C45:N45" si="6">+C15/(C$28*C$36)</f>
+        <f t="shared" ref="C45:N45" si="7">+C15/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75.592894601845444</v>
       </c>
       <c r="M45" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>62.945554705180392</v>
       </c>
       <c r="N45" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12.020815280171307</v>
       </c>
       <c r="P45" s="10" t="s">
         <v>5</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150.55926458719716</v>
       </c>
     </row>
@@ -7067,58 +7077,58 @@
         <v>4</v>
       </c>
       <c r="C46" s="11">
-        <f t="shared" ref="C46:N46" si="7">+C16/(C$28*C$36)</f>
+        <f t="shared" ref="C46:N46" si="8">+C16/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="K46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5118578920369088</v>
       </c>
       <c r="M46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N46" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P46" s="10" t="s">
         <v>4</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>101.51185789203691</v>
       </c>
     </row>
@@ -7127,58 +7137,58 @@
         <v>3</v>
       </c>
       <c r="C47" s="11">
-        <f t="shared" ref="C47:N47" si="8">+C17/(C$28*C$36)</f>
+        <f t="shared" ref="C47:N47" si="9">+C17/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>87.983358816150158</v>
       </c>
       <c r="I47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>101.77004891982148</v>
       </c>
       <c r="J47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="K47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N47" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P47" s="10" t="s">
         <v>3</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>229.75340773597162</v>
       </c>
     </row>
@@ -7187,51 +7197,51 @@
         <v>2</v>
       </c>
       <c r="C48" s="11">
-        <f t="shared" ref="C48:N48" si="9">+C18/(C$28*C$36)</f>
+        <f t="shared" ref="C48:N48" si="10">+C18/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>154.33694634917515</v>
       </c>
       <c r="E48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
       <c r="K48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.118578920369089</v>
       </c>
       <c r="M48" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N48" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P48" s="10" t="s">
@@ -7247,51 +7257,51 @@
         <v>1</v>
       </c>
       <c r="C49" s="14">
-        <f t="shared" ref="C49:N49" si="10">+C19/(C$28*C$36)</f>
+        <f t="shared" ref="C49:N49" si="11">+C19/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>80.178372573727316</v>
       </c>
       <c r="L49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M49" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N49" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P49" s="13" t="s">
@@ -7713,227 +7723,237 @@
         <v>35</v>
       </c>
       <c r="E64" s="2"/>
-      <c r="H64" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I64" s="2"/>
-      <c r="M64" s="2"/>
       <c r="R64" s="2"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B66" s="1" t="s">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>38</v>
+      </c>
+      <c r="H66" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I66" s="2"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="H67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1" t="s">
+      <c r="I67" s="1"/>
+      <c r="J67" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="K67" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B68" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="32">
+      <c r="C68" s="32">
         <v>16</v>
       </c>
-      <c r="D67" s="35">
+      <c r="D68" s="35">
         <v>1.8169999999999999</v>
       </c>
-      <c r="H67" s="28" t="s">
+      <c r="H68" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="I67" s="27"/>
-      <c r="J67" s="32">
+      <c r="I68" s="27"/>
+      <c r="J68" s="32">
         <v>16</v>
       </c>
-      <c r="K67" s="35">
+      <c r="K68" s="35">
         <v>1.9</v>
       </c>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B68" s="10" t="s">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B69" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C68" s="33">
+      <c r="C69" s="33">
         <v>44</v>
       </c>
-      <c r="D68" s="36">
+      <c r="D69" s="36">
         <v>1.411</v>
       </c>
-      <c r="H68" s="10" t="s">
+      <c r="H69" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="I68" s="12"/>
-      <c r="J68" s="33">
-        <v>44</v>
-      </c>
-      <c r="K68" s="36">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B69" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C69" s="33">
-        <v>28</v>
-      </c>
-      <c r="D69" s="36">
-        <v>1.0149999999999999</v>
-      </c>
-      <c r="H69" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="I69" s="12"/>
       <c r="J69" s="33">
+        <v>44</v>
+      </c>
+      <c r="K69" s="36">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B70" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" s="33">
         <v>28</v>
       </c>
-      <c r="K69" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B70" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C70" s="33">
-        <v>4</v>
-      </c>
-      <c r="D70" s="36"/>
+      <c r="D70" s="36">
+        <v>1.0149999999999999</v>
+      </c>
       <c r="H70" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I70" s="12"/>
       <c r="J70" s="33">
+        <v>28</v>
+      </c>
+      <c r="K70" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B71" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="33">
         <v>4</v>
       </c>
-      <c r="K70" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="L70" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B71" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" s="33">
-        <v>33</v>
-      </c>
-      <c r="D71" s="36">
-        <v>2.5710000000000002</v>
-      </c>
+      <c r="D71" s="36"/>
       <c r="H71" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I71" s="12"/>
       <c r="J71" s="33">
+        <v>4</v>
+      </c>
+      <c r="K71" s="36">
+        <v>0.8</v>
+      </c>
+      <c r="L71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B72" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K71" s="36">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L71" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B72" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="C72" s="33">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D72" s="36">
-        <v>2.0569999999999999</v>
+        <v>2.5710000000000002</v>
       </c>
       <c r="H72" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I72" s="12"/>
       <c r="J72" s="33">
+        <v>33</v>
+      </c>
+      <c r="K72" s="36">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B73" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K72" s="36">
-        <v>2</v>
-      </c>
-      <c r="L72" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B73" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="C73" s="33">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="D73" s="36">
-        <v>6.4160000000000004</v>
+        <v>2.0569999999999999</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I73" s="12"/>
       <c r="J73" s="33">
+        <v>31</v>
+      </c>
+      <c r="K73" s="36">
+        <v>2</v>
+      </c>
+      <c r="L73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B74" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="33">
         <v>60</v>
       </c>
-      <c r="K73" s="36">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B74" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C74" s="33">
-        <v>30</v>
-      </c>
       <c r="D74" s="36">
-        <v>2.7029999999999998</v>
+        <v>6.4160000000000004</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I74" s="12"/>
       <c r="J74" s="33">
+        <v>60</v>
+      </c>
+      <c r="K74" s="36">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B75" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C75" s="33">
         <v>30</v>
       </c>
-      <c r="K74" s="36">
+      <c r="D75" s="36">
+        <v>2.7029999999999998</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I75" s="12"/>
+      <c r="J75" s="33">
+        <v>30</v>
+      </c>
+      <c r="K75" s="36">
         <v>2.5</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B75" s="31" t="s">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B76" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C75" s="34">
+      <c r="C76" s="34">
         <v>18</v>
       </c>
-      <c r="D75" s="37">
+      <c r="D76" s="37">
         <v>0.96799999999999997</v>
       </c>
-      <c r="H75" s="31" t="s">
+      <c r="H76" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I75" s="15"/>
-      <c r="J75" s="34">
+      <c r="I76" s="15"/>
+      <c r="J76" s="34">
         <v>18</v>
       </c>
-      <c r="K75" s="37">
+      <c r="K76" s="37">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MadixKo More Formulas Added (Masses & Compound Names)
Added formulas that populate masses and compound names in the tables that follow the initial table.
</commit_message>
<xml_diff>
--- a/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
+++ b/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Github/MSRESOLVESG/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D0C7CFB-F7A1-46F2-975D-ABE12E056E6F}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE4F13B1-177E-44AB-8323-8B9191977A01}"/>
   <bookViews>
-    <workbookView xWindow="26445" yWindow="180" windowWidth="22605" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17295" yWindow="765" windowWidth="25260" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>Species</t>
   </si>
@@ -6066,8 +6066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6200,8 +6200,9 @@
         <v>0</v>
       </c>
       <c r="O12" s="11"/>
-      <c r="Q12" s="10" t="s">
-        <v>6</v>
+      <c r="Q12" s="10" t="str">
+        <f>$B12</f>
+        <v>methyl formate</v>
       </c>
       <c r="R12" s="16">
         <f>4+2*6+2*8</f>
@@ -6253,8 +6254,9 @@
         <v>0</v>
       </c>
       <c r="O13" s="11"/>
-      <c r="Q13" s="10" t="s">
-        <v>9</v>
+      <c r="Q13" s="10" t="str">
+        <f t="shared" ref="Q13:Q19" si="1">$B13</f>
+        <v>methanol-OD</v>
       </c>
       <c r="R13" s="16">
         <f>6+4+8</f>
@@ -6306,8 +6308,9 @@
         <v>0</v>
       </c>
       <c r="O14" s="11"/>
-      <c r="Q14" s="10" t="s">
-        <v>8</v>
+      <c r="Q14" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>methanol</v>
       </c>
       <c r="R14" s="16">
         <v>18</v>
@@ -6361,8 +6364,9 @@
         <v>17</v>
       </c>
       <c r="O15" s="11"/>
-      <c r="Q15" s="10" t="s">
-        <v>5</v>
+      <c r="Q15" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>methane</v>
       </c>
       <c r="R15" s="16">
         <v>10</v>
@@ -6416,8 +6420,9 @@
         <v>0</v>
       </c>
       <c r="O16" s="11"/>
-      <c r="Q16" s="10" t="s">
-        <v>4</v>
+      <c r="Q16" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>carbon monoxide</v>
       </c>
       <c r="R16" s="16">
         <v>14</v>
@@ -6471,8 +6476,9 @@
         <v>0</v>
       </c>
       <c r="O17" s="11"/>
-      <c r="Q17" s="10" t="s">
-        <v>3</v>
+      <c r="Q17" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>formaldehyde</v>
       </c>
       <c r="R17" s="16">
         <f>4+2+8</f>
@@ -6524,8 +6530,9 @@
         <v>0</v>
       </c>
       <c r="O18" s="11"/>
-      <c r="Q18" s="10" t="s">
-        <v>2</v>
+      <c r="Q18" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>carbon dioxide</v>
       </c>
       <c r="R18" s="16">
         <f>6+16</f>
@@ -6577,8 +6584,9 @@
         <v>0</v>
       </c>
       <c r="O19" s="11"/>
-      <c r="Q19" s="13" t="s">
-        <v>1</v>
+      <c r="Q19" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>water</v>
       </c>
       <c r="R19" s="26">
         <f>2+8</f>
@@ -6596,39 +6604,51 @@
         <v>16</v>
       </c>
       <c r="C27" s="8">
+        <f>C$11</f>
         <v>60</v>
       </c>
       <c r="D27" s="8">
+        <f t="shared" ref="D27:N27" si="2">D$11</f>
         <v>44</v>
       </c>
       <c r="E27" s="8">
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="F27" s="8">
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="G27" s="8">
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="H27" s="8">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="I27" s="8">
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="J27" s="8">
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="K27" s="8">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="L27" s="8">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M27" s="8">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N27" s="9">
+      <c r="N27" s="8">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="O27" s="16"/>
@@ -6642,47 +6662,47 @@
         <v>0.640400427119728</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" ref="D28:N28" si="1">IF(D27&lt;30,1,10^((30-D11)/155))</f>
+        <f t="shared" ref="D28:N28" si="3">IF(D27&lt;30,1,10^((30-D11)/155))</f>
         <v>0.81222699470800896</v>
       </c>
       <c r="E28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.95641231880567645</v>
       </c>
       <c r="F28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.9707262508693274</v>
       </c>
       <c r="G28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.98525440921080254</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O28" s="17"/>
@@ -6692,39 +6712,51 @@
         <v>16</v>
       </c>
       <c r="C35" s="8">
+        <f>C$11</f>
         <v>60</v>
       </c>
       <c r="D35" s="8">
+        <f t="shared" ref="D35:N35" si="4">D$11</f>
         <v>44</v>
       </c>
       <c r="E35" s="8">
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="F35" s="8">
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="G35" s="8">
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="H35" s="8">
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="I35" s="8">
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="J35" s="8">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="K35" s="8">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="L35" s="8">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="M35" s="8">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="N35" s="9">
+      <c r="N35" s="8">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="O35" s="16"/>
@@ -6734,51 +6766,51 @@
         <v>14</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" ref="C36:N36" si="2">+(28/C11)^(0.5)</f>
+        <f t="shared" ref="C36:N36" si="5">+(28/C11)^(0.5)</f>
         <v>0.68313005106397318</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.7977240352174656</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.92113237294367656</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.93541434669348533</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.95038192662298293</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.96609178307929588</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.98260736888103495</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.247219128924647</v>
       </c>
       <c r="L36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.3228756555322954</v>
       </c>
       <c r="M36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.3662601021279464</v>
       </c>
       <c r="N36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="O36" s="4"/>
@@ -6837,51 +6869,51 @@
         <v>6</v>
       </c>
       <c r="C42" s="11">
-        <f t="shared" ref="C42:N42" si="3">+C12/(C$28*C$36)</f>
+        <f t="shared" ref="C42:N42" si="6">+C12/(C$28*C$36)</f>
         <v>68.575068696001424</v>
       </c>
       <c r="D42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>44.05134678050878</v>
       </c>
       <c r="G42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>106.79562068249264</v>
       </c>
       <c r="H42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>11.386081729148845</v>
       </c>
       <c r="I42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>69.203633265478615</v>
       </c>
       <c r="J42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="K42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>21.957751641341996</v>
       </c>
       <c r="N42" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P42" s="28" t="s">
@@ -6897,58 +6929,58 @@
         <v>9</v>
       </c>
       <c r="C43" s="11">
-        <f t="shared" ref="C43:N43" si="4">+C13/(C$28*C$36)</f>
+        <f t="shared" ref="C43:N43" si="7">+C13/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>89.672625238771516</v>
       </c>
       <c r="F43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>110.12836695127194</v>
       </c>
       <c r="G43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.2038686204747795</v>
       </c>
       <c r="H43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.3158850511217821</v>
       </c>
       <c r="I43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>18.318608805567866</v>
       </c>
       <c r="J43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M43" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.3192505471139997</v>
       </c>
       <c r="N43" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P43" s="10" t="s">
         <v>9</v>
       </c>
       <c r="Q43">
-        <f t="shared" ref="Q43:Q47" si="5">+SUM(C43:N43)</f>
+        <f t="shared" ref="Q43:Q47" si="8">+SUM(C43:N43)</f>
         <v>237.95860521432189</v>
       </c>
     </row>
@@ -6957,58 +6989,58 @@
         <v>8</v>
       </c>
       <c r="C44" s="11">
-        <f t="shared" ref="C44:N44" si="6">+C14/(C$28*C$36)</f>
+        <f t="shared" ref="C44:N44" si="9">+C14/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>79.292424204915804</v>
       </c>
       <c r="G44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>106.79562068249264</v>
       </c>
       <c r="H44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3.1052950170405942</v>
       </c>
       <c r="I44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>42.743420546325019</v>
       </c>
       <c r="J44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="K44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N44" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P44" s="10" t="s">
         <v>8</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>240.93676045077405</v>
       </c>
     </row>
@@ -7017,58 +7049,58 @@
         <v>5</v>
       </c>
       <c r="C45" s="11">
-        <f t="shared" ref="C45:N45" si="7">+C15/(C$28*C$36)</f>
+        <f t="shared" ref="C45:N45" si="10">+C15/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>75.592894601845444</v>
       </c>
       <c r="M45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>62.945554705180392</v>
       </c>
       <c r="N45" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>12.020815280171307</v>
       </c>
       <c r="P45" s="10" t="s">
         <v>5</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>150.55926458719716</v>
       </c>
     </row>
@@ -7077,58 +7109,58 @@
         <v>4</v>
       </c>
       <c r="C46" s="11">
-        <f t="shared" ref="C46:N46" si="8">+C16/(C$28*C$36)</f>
+        <f t="shared" ref="C46:N46" si="11">+C16/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>100</v>
       </c>
       <c r="K46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.5118578920369088</v>
       </c>
       <c r="M46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N46" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P46" s="10" t="s">
         <v>4</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>101.51185789203691</v>
       </c>
     </row>
@@ -7137,58 +7169,58 @@
         <v>3</v>
       </c>
       <c r="C47" s="11">
-        <f t="shared" ref="C47:N47" si="9">+C17/(C$28*C$36)</f>
+        <f t="shared" ref="C47:N47" si="12">+C17/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>87.983358816150158</v>
       </c>
       <c r="I47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>101.77004891982148</v>
       </c>
       <c r="J47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
       <c r="K47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M47" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N47" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P47" s="10" t="s">
         <v>3</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>229.75340773597162</v>
       </c>
     </row>
@@ -7197,51 +7229,51 @@
         <v>2</v>
       </c>
       <c r="C48" s="11">
-        <f t="shared" ref="C48:N48" si="10">+C18/(C$28*C$36)</f>
+        <f t="shared" ref="C48:N48" si="13">+C18/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>154.33694634917515</v>
       </c>
       <c r="E48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="K48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>15.118578920369089</v>
       </c>
       <c r="M48" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N48" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P48" s="10" t="s">
@@ -7257,51 +7289,51 @@
         <v>1</v>
       </c>
       <c r="C49" s="14">
-        <f t="shared" ref="C49:N49" si="11">+C19/(C$28*C$36)</f>
+        <f t="shared" ref="C49:N49" si="14">+C19/(C$28*C$36)</f>
         <v>0</v>
       </c>
       <c r="D49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>80.178372573727316</v>
       </c>
       <c r="L49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M49" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N49" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P49" s="13" t="s">
@@ -7322,47 +7354,60 @@
         <v>0</v>
       </c>
       <c r="C53" s="8">
+        <f>C$11</f>
         <v>60</v>
       </c>
       <c r="D53" s="8">
+        <f t="shared" ref="D53:N53" si="15">D$11</f>
         <v>44</v>
       </c>
       <c r="E53" s="8">
+        <f t="shared" si="15"/>
         <v>33</v>
       </c>
       <c r="F53" s="8">
+        <f t="shared" si="15"/>
         <v>32</v>
       </c>
       <c r="G53" s="8">
+        <f t="shared" si="15"/>
         <v>31</v>
       </c>
       <c r="H53" s="8">
+        <f t="shared" si="15"/>
         <v>30</v>
       </c>
       <c r="I53" s="8">
+        <f t="shared" si="15"/>
         <v>29</v>
       </c>
       <c r="J53" s="8">
+        <f t="shared" si="15"/>
         <v>28</v>
       </c>
       <c r="K53" s="8">
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
       <c r="L53" s="8">
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
       <c r="M53" s="8">
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
-      <c r="N53" s="9">
+      <c r="N53" s="8">
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
       <c r="O53"/>
       <c r="R53" s="2"/>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B54" s="10" t="s">
-        <v>6</v>
+      <c r="B54" s="10" t="str">
+        <f>$B12</f>
+        <v>methyl formate</v>
       </c>
       <c r="C54" s="18">
         <f>+ $Q42/($S12*C12)</f>
@@ -7409,8 +7454,9 @@
       </c>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="10" t="s">
-        <v>9</v>
+      <c r="B55" s="10" t="str">
+        <f t="shared" ref="B55:B61" si="16">$B13</f>
+        <v>methanol-OD</v>
       </c>
       <c r="C55" s="18">
         <v>0</v>
@@ -7456,8 +7502,9 @@
       </c>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="10" t="s">
-        <v>8</v>
+      <c r="B56" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>methanol</v>
       </c>
       <c r="C56" s="18">
         <v>0</v>
@@ -7502,8 +7549,9 @@
       </c>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B57" s="10" t="s">
-        <v>5</v>
+      <c r="B57" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>methane</v>
       </c>
       <c r="C57" s="18">
         <v>0</v>
@@ -7546,8 +7594,9 @@
       </c>
     </row>
     <row r="58" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
-        <v>4</v>
+      <c r="B58" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>carbon monoxide</v>
       </c>
       <c r="C58" s="18">
         <v>0</v>
@@ -7589,8 +7638,9 @@
       </c>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="10" t="s">
-        <v>3</v>
+      <c r="B59" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>formaldehyde</v>
       </c>
       <c r="C59" s="18">
         <v>0</v>
@@ -7633,8 +7683,9 @@
       </c>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B60" s="10" t="s">
-        <v>2</v>
+      <c r="B60" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>carbon dioxide</v>
       </c>
       <c r="C60" s="18">
         <v>0</v>
@@ -7677,8 +7728,9 @@
       </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B61" s="13" t="s">
-        <v>1</v>
+      <c r="B61" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>water</v>
       </c>
       <c r="C61" s="20">
         <v>0</v>

</xml_diff>

<commit_message>
MadixKo & Manual Update Version 0.0
Added MadixKo equation to MadixKo Excel Sheet. Updated Manual, changed "Signal Relative to CO" to "Concentration Relative to CO" in the MadixKo equation.
</commit_message>
<xml_diff>
--- a/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
+++ b/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Github/MSRESOLVESG/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE4F13B1-177E-44AB-8323-8B9191977A01}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFF245D8-EC7C-461B-A874-D933EDA5D896}"/>
   <bookViews>
-    <workbookView xWindow="17295" yWindow="765" windowWidth="25260" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27975" yWindow="330" windowWidth="28455" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>Species</t>
   </si>
@@ -152,12 +152,65 @@
   <si>
     <t>The below table(s) were manually populated from the above table.</t>
   </si>
+  <si>
+    <t>Relationship used:</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* Concetration = Signal </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Signal * C = Concetration</t>
+    </r>
+  </si>
+  <si>
+    <t>Below represents the MadixKo equation used:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +236,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="15"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -409,6 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5740,6 +5817,56 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1648520</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>19280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A165D47C-52FE-425F-BA74-97C7E15567E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11811000" y="10734675"/>
+          <a:ext cx="4982270" cy="1648055"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6066,8 +6193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O81" sqref="O81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6086,7 +6213,7 @@
     <col min="13" max="13" width="9" customWidth="1"/>
     <col min="14" max="15" width="11.7109375" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.28515625" customWidth="1"/>
     <col min="20" max="20" width="26.5703125" customWidth="1"/>
   </cols>
@@ -7777,7 +7904,12 @@
       <c r="E64" s="2"/>
       <c r="R64" s="2"/>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="Q65" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>38</v>
       </c>
@@ -7792,7 +7924,7 @@
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
@@ -7813,7 +7945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B68" s="28" t="s">
         <v>29</v>
       </c>
@@ -7834,7 +7966,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
         <v>28</v>
       </c>
@@ -7855,7 +7987,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
         <v>30</v>
       </c>
@@ -7876,7 +8008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="s">
         <v>34</v>
       </c>
@@ -7898,7 +8030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B72" s="10" t="s">
         <v>33</v>
       </c>
@@ -7922,7 +8054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B73" s="10" t="s">
         <v>31</v>
       </c>
@@ -7946,7 +8078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B74" s="10" t="s">
         <v>32</v>
       </c>
@@ -7967,7 +8099,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B75" s="10" t="s">
         <v>36</v>
       </c>
@@ -7988,7 +8120,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:20" ht="21.75" x14ac:dyDescent="0.3">
       <c r="B76" s="31" t="s">
         <v>27</v>
       </c>
@@ -8008,6 +8140,14 @@
       <c r="K76" s="37">
         <v>1</v>
       </c>
+      <c r="Q76" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="R76" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="S76" s="39"/>
+      <c r="T76" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Manual SLS README Revamped
</commit_message>
<xml_diff>
--- a/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
+++ b/Documentation/180613MadixKoMSCorrectionsFactorExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Github/MSRESOLVESG/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA5B7668-8939-44B5-85AF-67D6150565D5}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{4E9C3DC8-730E-4252-99E4-88B093BCAD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{045C10E9-E199-4F7E-B11E-D4CB2461FB22}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="28800" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21435" yWindow="1080" windowWidth="27495" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -6194,8 +6193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q79" sqref="Q79"/>
+    <sheetView tabSelected="1" topLeftCell="E56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N76" sqref="N76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>